<commit_message>
Entrenamiento y Simulacion listo
</commit_message>
<xml_diff>
--- a/DATA/OUT/EJEMPLO_4.xlsx
+++ b/DATA/OUT/EJEMPLO_4.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,16 +449,16 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>YD1</t>
+          <t>X3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -466,24 +466,24 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -491,32 +491,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -530,7 +508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,12 +525,17 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.9498716502627649</v>
+        <v>0.7226984551978297</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-4.747000061854188</v>
+        <v>0.8104254099121104</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-0.7706304189360769</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +566,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-5.396852785246973</v>
+        <v>0.6694997070989952</v>
       </c>
     </row>
   </sheetData>
@@ -615,7 +598,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SIGMOIDE</t>
+          <t>ESCALON</t>
         </is>
       </c>
     </row>

</xml_diff>